<commit_message>
Add Tarefas.txt and Problemas.txt
</commit_message>
<xml_diff>
--- a/Documentos/Caraterísticas.xlsx
+++ b/Documentos/Caraterísticas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Produto</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Lista SOS</t>
+  </si>
+  <si>
+    <t>Casa</t>
   </si>
 </sst>
 </file>
@@ -489,7 +492,7 @@
   <dimension ref="B2:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,18 +513,21 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -532,13 +538,16 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>43187</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>